<commit_message>
reportNG with ststic screenshot implemented and also CustomListers added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\DataDrivenFramework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse_projects\Data-Driven-Framework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202E21F-03A0-4316-ACAA-1AF86F7FE3B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="3540" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,10 +24,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>postCode</t>
+  </si>
+  <si>
+    <t>Sohaib</t>
+  </si>
+  <si>
+    <t>Majeed</t>
+  </si>
+  <si>
+    <t>123wp</t>
+  </si>
+  <si>
+    <t>alertText</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,13 +374,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new files for CUstomListeners and excel file for data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse_projects\Data-Driven-Framework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4202E21F-03A0-4316-ACAA-1AF86F7FE3B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CF257A-1BF4-4EAC-A3C5-90A3B0EF817D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,14 +378,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Data Driven Framework course completed except Jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse_projects\Data-Driven-Framework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CF257A-1BF4-4EAC-A3C5-90A3B0EF817D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="2160" windowWidth="15375" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="addCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="openAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>lastName</t>
   </si>
@@ -49,12 +50,75 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Daniyal</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Kashan</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Usman</t>
+  </si>
+  <si>
+    <t>Shabeer</t>
+  </si>
+  <si>
+    <t>4567xy</t>
+  </si>
+  <si>
+    <t>76yrt</t>
+  </si>
+  <si>
+    <t>89rt</t>
+  </si>
+  <si>
+    <t>Sohaib Majeed</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>runMode</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,11 +438,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +452,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -401,8 +465,11 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -414,6 +481,147 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ignore un nexessary files and pull new changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eclipse_projects\Data-Driven-Framework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CF257A-1BF4-4EAC-A3C5-90A3B0EF817D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="2160" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="2160" windowWidth="15375" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="addCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="openAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>lastName</t>
   </si>
@@ -49,12 +50,72 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Daniyal</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Kashan</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Usman</t>
+  </si>
+  <si>
+    <t>Shabeer</t>
+  </si>
+  <si>
+    <t>4567xy</t>
+  </si>
+  <si>
+    <t>76yrt</t>
+  </si>
+  <si>
+    <t>89rt</t>
+  </si>
+  <si>
+    <t>Sohaib Majeed</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>runMode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,11 +435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +449,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -401,8 +462,11 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -414,6 +478,147 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>